<commit_message>
effect table sub_type_key/vale -> sub_type으로 간소화
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/이전목록.xlsx
+++ b/로스트아크/데이터테이블/이전목록.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335EFB4D-CC41-443F-A23E-B4A1A8AE7CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72384C4B-638B-4BE2-8C44-B16B05D6DCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3444" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설명" sheetId="2" r:id="rId1"/>
     <sheet name="목록" sheetId="1" r:id="rId2"/>
     <sheet name="트라이포드 인포" sheetId="3" r:id="rId3"/>
     <sheet name="스킬 리소스" sheetId="4" r:id="rId4"/>
+    <sheet name="effect table schema" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="201">
   <si>
     <t>icon_res</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -669,6 +670,748 @@
   </si>
   <si>
     <t>lm_skill_27_sound.wav</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect Table Schema</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>칼럼명</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료형</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>효과 요약 설명 (기획용)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>효과 ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>효과 명칭</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">효과의 종류  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 일반 효과 (DEFAULT)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 버프 등 이로운 효과(BUFF) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 디버프 등 해로운 효과 (DEBUFF)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">효과의 유형  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 피해형(DAMAGE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 능력치 조절(STAT)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 특수 기능(SPECIAL) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 스킬 제어(SKILL_CONTROL) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 오브젝트 제어(OBJECT_CONTROL)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">type별 상세 효과 유형 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(아래의 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[비고 1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 참고)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply_type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">효과가 적용되는 방식  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 대미지 처리(DEAL)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 고정 수치 증가(PLUS)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 비율 증가(INCREASE) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 고정 수치 감소(MINUS) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 비율 감소(DECREASE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 부여(GRANT) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 변경 (CHANGE) </t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[비고 1] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type별 상세 효과</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type = 0 (피해형)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = dealing_type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>direct</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type = 1 (능력치 조절)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = target_stat</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type = 2 (특수 기능)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = immune_type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = buff_type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = hit_reaction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = debuff_type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type = 3 (스킬 제어)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = skill_attribute</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type = 4 (오브젝트 제어)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_type = object_type</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -681,7 +1424,7 @@
     <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="0.0&quot;, &quot;0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,8 +1506,68 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="4"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF0070C0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,8 +1592,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -828,11 +1655,294 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -891,14 +2001,107 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1232,7 +2435,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1241,34 +2444,34 @@
       <c r="D3" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="22" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B4" s="20"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B5" s="20"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="3" t="s">
         <v>124</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2276,15 +3479,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813847DB-15CC-479F-8F4D-BBB6A106FEB8}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.69921875" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.19921875" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2300,112 +3503,112 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2413,4 +3616,485 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7274176-EBDE-47A4-9780-EFC67E94975C}">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="107.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="23"/>
+      <c r="B3" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="23"/>
+      <c r="B4" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="36">
+        <f>ROW(B5)-4</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="23"/>
+      <c r="B6" s="40">
+        <f t="shared" ref="B6:B10" si="0">ROW(B6)-4</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="31"/>
+    </row>
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.4">
+      <c r="A7" s="23"/>
+      <c r="B7" s="40">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="31"/>
+    </row>
+    <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.4">
+      <c r="A8" s="23"/>
+      <c r="B8" s="40">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="31"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="23"/>
+      <c r="B9" s="40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" s="31"/>
+    </row>
+    <row r="10" spans="1:6" ht="37.200000000000003" x14ac:dyDescent="0.4">
+      <c r="A10" s="23"/>
+      <c r="B10" s="40">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="23"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="23"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="23"/>
+      <c r="B14" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="23"/>
+      <c r="B15" s="51">
+        <v>1</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" s="23"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="23"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="23"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="23"/>
+      <c r="B19" s="51">
+        <v>2</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="23"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="23"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="23"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="23"/>
+      <c r="B23" s="51">
+        <v>3</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="52"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="23"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="23"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="23"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" s="23"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" s="23"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" s="23"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="23"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" s="23"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" s="23"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" s="23"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A34" s="23"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="23"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="23"/>
+      <c r="B36" s="51">
+        <v>4</v>
+      </c>
+      <c r="C36" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" s="52"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37" s="23"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38" s="23"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="23"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="23"/>
+      <c r="B40" s="51">
+        <v>5</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" s="52"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A41" s="23"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42" s="23"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B14:D14"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>